<commit_message>
embed resourcePermissions in course
</commit_message>
<xml_diff>
--- a/xxx/x-ui/ui-v1.xlsx
+++ b/xxx/x-ui/ui-v1.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jag/jag/JUNIVERSE/WS/jag-saas/xxx/x-ui/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{47CA4FFE-9900-FB4D-99F9-22EB0E3B73CF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{20F36E49-2368-A343-B0DE-4486E0C8E968}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="27460" windowHeight="17040" xr2:uid="{075031BD-FBDA-1B4E-8EDE-27C85E1E4A07}"/>
   </bookViews>
   <sheets>
-    <sheet name="User Admin" sheetId="1" r:id="rId1"/>
+    <sheet name="UserAdmin-UserPermission" sheetId="5" r:id="rId1"/>
+    <sheet name="UserAdmin-UserList" sheetId="1" r:id="rId2"/>
+    <sheet name="UserAdmin-UserDetails" sheetId="3" r:id="rId3"/>
+    <sheet name="UserAdmin-CreateUser" sheetId="2" r:id="rId4"/>
+    <sheet name="UserAdmin-UpdateUser" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,9 +28,77 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>CREATE_USER</t>
+  </si>
+  <si>
+    <t>READ_ANY_USER</t>
+  </si>
+  <si>
+    <t>UPDATE_ANY_USER</t>
+  </si>
+  <si>
+    <t>DELETE_ANY_USER</t>
+  </si>
+  <si>
+    <t>CREATE_USER_GROUP</t>
+  </si>
+  <si>
+    <t>USER_GROUP</t>
+  </si>
+  <si>
+    <t>READ_ANY_USER_GROUP</t>
+  </si>
+  <si>
+    <t>UPDATE_ANY_USER_GROUP</t>
+  </si>
+  <si>
+    <t>DELETE_ANY_USER_GROUP</t>
+  </si>
+  <si>
+    <t>CREATE_COURSE</t>
+  </si>
+  <si>
+    <t>COURSE</t>
+  </si>
+  <si>
+    <t>READ_ANY_COURSE</t>
+  </si>
+  <si>
+    <t>UPDATE_ANY_COURSE</t>
+  </si>
+  <si>
+    <t>DELETE_ANY_COURSE</t>
+  </si>
+  <si>
+    <t>CUSTOM_ACCESS1_COURSE</t>
+  </si>
+  <si>
+    <t>CREATE_COURSE_GROUP</t>
+  </si>
+  <si>
+    <t>READ_ANY_COURSE_GROUP</t>
+  </si>
+  <si>
+    <t>UPDATE_ANY_COURSE_GROUP</t>
+  </si>
+  <si>
+    <t>DELETE_ANY_COURSE_GROUP</t>
+  </si>
+  <si>
+    <t>COURSE_GROUP</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -34,13 +106,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -55,8 +156,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,10 +474,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{983D049A-8D9A-B14E-A125-CCB95A39F7DD}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885E661D-6971-4446-97C5-36AEE796A691}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -381,4 +617,46 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E526501-5953-474F-A0A4-52B07D792E2B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587FAA9C-E52C-5844-8778-758AB89774DF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3B4FC2F-BADB-4240-B5FB-B197F7DA41EC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>